<commit_message>
finished highshooter code with kicker and indicator light for ball
</commit_message>
<xml_diff>
--- a/CompetitionCode/MotorMap.xlsx
+++ b/CompetitionCode/MotorMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>PWM 0</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>LoadWheel</t>
+  </si>
+  <si>
+    <t>DIO:</t>
+  </si>
+  <si>
+    <t>PhotoEye for Gear</t>
+  </si>
+  <si>
+    <t>ball sensor</t>
+  </si>
+  <si>
+    <t>ball indicator</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,59 +455,89 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
         <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated addresses on SRX. First test
drive works (including switiching of forward direction).
climber works (limit switch for top is 'reverse')
intake works (and stop 2s after changing direction)
</commit_message>
<xml_diff>
--- a/CompetitionCode/MotorMap.xlsx
+++ b/CompetitionCode/MotorMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>PWM 0</t>
   </si>
@@ -69,6 +69,21 @@
   </si>
   <si>
     <t>ball indicator</t>
+  </si>
+  <si>
+    <t>climber master</t>
+  </si>
+  <si>
+    <t>lifter</t>
+  </si>
+  <si>
+    <t>climber slave</t>
+  </si>
+  <si>
+    <t>shooter</t>
+  </si>
+  <si>
+    <t>collector stirrer</t>
   </si>
 </sst>
 </file>
@@ -420,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,6 +479,9 @@
       <c r="A6">
         <v>1</v>
       </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -501,38 +519,60 @@
       <c r="A11">
         <v>6</v>
       </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>7</v>
       </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="A14">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>1</v>
-      </c>
-      <c r="B16" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>2</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
tested pneumatic and servo camera
</commit_message>
<xml_diff>
--- a/CompetitionCode/MotorMap.xlsx
+++ b/CompetitionCode/MotorMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>PWM 0</t>
   </si>
@@ -68,9 +68,6 @@
     <t>ball sensor</t>
   </si>
   <si>
-    <t>ball indicator</t>
-  </si>
-  <si>
     <t>climber master</t>
   </si>
   <si>
@@ -84,6 +81,12 @@
   </si>
   <si>
     <t>collector stirrer</t>
+  </si>
+  <si>
+    <t>climbpos2</t>
+  </si>
+  <si>
+    <t>climbpos1</t>
   </si>
 </sst>
 </file>
@@ -435,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +483,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,7 +523,7 @@
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -528,7 +531,7 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -536,7 +539,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -544,7 +547,7 @@
         <v>9</v>
       </c>
       <c r="B14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -573,7 +576,15 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto find peg tested. guitar control. tweaks
</commit_message>
<xml_diff>
--- a/CompetitionCode/MotorMap.xlsx
+++ b/CompetitionCode/MotorMap.xlsx
@@ -440,8 +440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>